<commit_message>
Revert "덕진 - 금요일"
This reverts commit ca48ddcf723af2045c8e34cf76481c3ae836dc99.
</commit_message>
<xml_diff>
--- a/울산, 수원 처리불량건.xlsx
+++ b/울산, 수원 처리불량건.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="300">
   <si>
     <t>모   델</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1208,9 +1208,6 @@
   </si>
   <si>
     <t>POL43U</t>
-  </si>
-  <si>
-    <t>이애순</t>
   </si>
 </sst>
 </file>
@@ -3563,7 +3560,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4657,12 +4654,12 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
+    <col min="1" max="1" width="8.375" customWidth="1"/>
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="22.75" customWidth="1"/>
     <col min="4" max="4" width="12.875" customWidth="1"/>
@@ -4727,21 +4724,11 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C4" s="15">
-        <v>43804</v>
-      </c>
-      <c r="D4" s="2">
-        <v>201019</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>284</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Revert "Revert "덕진 - 금요일""
This reverts commit 8d0fdd2281784cf91657c60b83d0f9c1ec75cfaf.
</commit_message>
<xml_diff>
--- a/울산, 수원 처리불량건.xlsx
+++ b/울산, 수원 처리불량건.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="301">
   <si>
     <t>모   델</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1208,6 +1208,9 @@
   </si>
   <si>
     <t>POL43U</t>
+  </si>
+  <si>
+    <t>이애순</t>
   </si>
 </sst>
 </file>
@@ -3560,7 +3563,7 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4654,12 +4657,12 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
     <col min="2" max="2" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="22.75" customWidth="1"/>
     <col min="4" max="4" width="12.875" customWidth="1"/>
@@ -4724,11 +4727,21 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="15">
+        <v>43804</v>
+      </c>
+      <c r="D4" s="2">
+        <v>201019</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>284</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>